<commit_message>
add - management command - insert employee by excel
</commit_message>
<xml_diff>
--- a/core/seed_employees_employeejobspecialty.xlsx
+++ b/core/seed_employees_employeejobspecialty.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan.cheng\Documents\Visual Studio Code\Django\p_sys01_repo01\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20763F44-8CCB-4F4A-B257-316160C1598A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1869A31-C54A-4138-B92F-F35765DBC485}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>NAME</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>SPEC 15</t>
+  </si>
+  <si>
+    <t>ACCOUNTING</t>
+  </si>
+  <si>
+    <t>BILLING</t>
   </si>
 </sst>
 </file>
@@ -950,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A30"/>
+  <dimension ref="A1:A32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1035,76 +1041,86 @@
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>